<commit_message>
Final  submitted code and Report
</commit_message>
<xml_diff>
--- a/SP1/Report.xlsx
+++ b/SP1/Report.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="20">
   <si>
     <t>mergeSort(int)</t>
   </si>
@@ -64,6 +64,21 @@
   </si>
   <si>
     <t>12901 msec.</t>
+  </si>
+  <si>
+    <t>insertionSort(Integers)</t>
+  </si>
+  <si>
+    <t>&gt; 2 min</t>
+  </si>
+  <si>
+    <t>13 msec.</t>
+  </si>
+  <si>
+    <t>28 msec.</t>
+  </si>
+  <si>
+    <t>617 msec.</t>
   </si>
 </sst>
 </file>
@@ -87,7 +102,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -95,12 +110,106 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -409,94 +518,131 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:C8"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="A2" sqref="A2:D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="16.90625" customWidth="1"/>
-    <col min="2" max="2" width="13" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.54296875" customWidth="1"/>
+    <col min="2" max="2" width="14.26953125" customWidth="1"/>
     <col min="3" max="3" width="17.6328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+    <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A3">
+      <c r="D2" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" s="10">
+        <v>10000</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="4">
         <v>1000000</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B4" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C4" s="5" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A4">
+      <c r="D4" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5" s="4">
         <v>2000000</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B5" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C5" s="5" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A5">
+      <c r="D5" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6" s="4">
         <v>5000000</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B6" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C6" s="5" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A6">
+      <c r="D6" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A7" s="4">
         <v>6000000</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B7" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C7" s="5" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A7">
+      <c r="D7" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A8" s="4">
         <v>10000000</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B8" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C8" s="5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A8">
+      <c r="D8" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A9" s="7">
         <v>15000000</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B9" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C9" s="8" t="s">
         <v>14</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>